<commit_message>
SpreadSheets and R Scripts
</commit_message>
<xml_diff>
--- a/Excel/CRQ2_2.xlsx
+++ b/Excel/CRQ2_2.xlsx
@@ -464,11 +464,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:XFD74"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="34" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="34.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>